<commit_message>
worksheet range now dynamic, depends only on filled cells in ws
</commit_message>
<xml_diff>
--- a/KeremetForms/Template/example.xlsx
+++ b/KeremetForms/Template/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\C#\KeremetForms\KeremetForms\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASerikov.KGBANK\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -265,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -281,8 +281,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -566,7 +564,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +628,7 @@
       <c r="E4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="14" t="s">
@@ -647,7 +645,7 @@
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>